<commit_message>
developed structure around placing an order some more
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/VendorsAndProducts.xlsx
+++ b/Project0/TempMohit/Data/VendorsAndProducts.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project0\Damle_M_Valentine_N_P0\Project0\TempMohit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7EFF0F-6EC1-4D2A-93CA-838DC5F07B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EF7CFC-834D-47BB-A64B-7170F684E7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VenderList" sheetId="1" r:id="rId1"/>
+    <sheet name="VendorList" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="2" r:id="rId2"/>
-    <sheet name="OrderListProcessed" sheetId="3" r:id="rId3"/>
+    <sheet name="OrdersPlaced" sheetId="3" r:id="rId3"/>
+    <sheet name="OrderClientRef" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Vendor</t>
   </si>
@@ -72,6 +73,21 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Full Price</t>
+  </si>
+  <si>
+    <t>Final Price</t>
+  </si>
+  <si>
+    <t>Order Id</t>
+  </si>
+  <si>
+    <t>Client Id</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -541,15 +557,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5932EE45-03E0-47C7-8810-8C80A94F3D73}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -560,70 +576,82 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -632,4 +660,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5A07BB-59BC-4B37-8F44-1FFF68603EF7}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="A2:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
figuring out how to manipulate data columns for place order
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/VendorsAndProducts.xlsx
+++ b/Project0/TempMohit/Data/VendorsAndProducts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project0\Damle_M_Valentine_N_P0\Project0\TempMohit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EF7CFC-834D-47BB-A64B-7170F684E7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DED5728-AE5B-405E-811C-560283DA93DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,12 +75,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Full Price</t>
-  </si>
-  <si>
-    <t>Final Price</t>
-  </si>
-  <si>
     <t>Order Id</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>FullPrice</t>
+  </si>
+  <si>
+    <t>FinalPrice</t>
   </si>
 </sst>
 </file>
@@ -560,7 +560,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,19 +576,19 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -674,10 +674,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on place order feature: trying to get sequence to determine an order id for the current order being placed
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/VendorsAndProducts.xlsx
+++ b/Project0/TempMohit/Data/VendorsAndProducts.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project0\Damle_M_Valentine_N_P0\Project0\TempMohit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DED5728-AE5B-405E-811C-560283DA93DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C27247-7308-4943-8260-05845145E363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VendorList" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="2" r:id="rId2"/>
     <sheet name="OrdersPlaced" sheetId="3" r:id="rId3"/>
-    <sheet name="OrderClientRef" sheetId="4" r:id="rId4"/>
+    <sheet name="OrderReference" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Vendor</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>FinalPrice</t>
+  </si>
+  <si>
+    <t>TotalExpense</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5932EE45-03E0-47C7-8810-8C80A94F3D73}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -664,20 +667,43 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5A07BB-59BC-4B37-8F44-1FFF68603EF7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="A2:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mvp feature: place order: finished component that appends a placed order summaries Excel sheet
</commit_message>
<xml_diff>
--- a/Project0/TempMohit/Data/VendorsAndProducts.xlsx
+++ b/Project0/TempMohit/Data/VendorsAndProducts.xlsx
@@ -8,15 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project0\Damle_M_Valentine_N_P0\Project0\TempMohit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C27247-7308-4943-8260-05845145E363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC0F4DF-529E-46E1-8961-3D5D74F24D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VendorList" sheetId="1" r:id="rId1"/>
     <sheet name="ProductList" sheetId="2" r:id="rId2"/>
-    <sheet name="OrdersPlaced" sheetId="3" r:id="rId3"/>
-    <sheet name="OrderReference" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Vendor</t>
   </si>
@@ -51,6 +49,9 @@
     <t>Discount</t>
   </si>
   <si>
+    <t>InStock</t>
+  </si>
+  <si>
     <t>milk</t>
   </si>
   <si>
@@ -67,30 +68,6 @@
   </si>
   <si>
     <t>rain jacket</t>
-  </si>
-  <si>
-    <t>OrderId</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Order Id</t>
-  </si>
-  <si>
-    <t>Client Id</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>FullPrice</t>
-  </si>
-  <si>
-    <t>FinalPrice</t>
-  </si>
-  <si>
-    <t>TotalExpense</t>
   </si>
 </sst>
 </file>
@@ -447,15 +424,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC12278D-B496-49FA-95A5-08884BF45119}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9 D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10 E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -468,10 +445,13 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>2.99</v>
@@ -482,10 +462,13 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>1.29</v>
@@ -496,10 +479,13 @@
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -510,10 +496,13 @@
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>15</v>
@@ -524,10 +513,13 @@
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1">
         <v>3.99</v>
@@ -538,10 +530,13 @@
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>21</v>
@@ -552,158 +547,8 @@
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5932EE45-03E0-47C7-8810-8C80A94F3D73}">
-  <dimension ref="A1:H12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5A07BB-59BC-4B37-8F44-1FFF68603EF7}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="E7" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>